<commit_message>
fixed book incorrect answer 11th botancy
</commit_message>
<xml_diff>
--- a/tamil_biology/XIth_BIO-BOTANY_TM_Combined-Page_326-336.xlsx
+++ b/tamil_biology/XIth_BIO-BOTANY_TM_Combined-Page_326-336.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\2020\git\tvmani.github.io\tamil_biology\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC7583AD-F7A9-4518-82C2-E8193253DFD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72B408D1-6DAB-4EE6-AD24-28B1F9637A3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="11964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1123" uniqueCount="792">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1122" uniqueCount="791">
   <si>
     <t>question_no</t>
   </si>
@@ -2367,15 +2367,6 @@
   </si>
   <si>
     <t>மொட்டு விடுதல்</t>
-  </si>
-  <si>
-    <t xml:space="preserve">கீழே கொடுக்கப்பட்டுள்ள (அ முதல் உ) கூற்றுகளை படித்து சரியான கூற்றுகளைக் கொண்ட பொருத்தமான விடையைத் தேர்ந்தெடுக்கவும். 
-அ) மாஸ்களும், லைக்கென்களும் வெற்றுப்பாறைகளில் கூட்டமாக வாழும் முதல் உயிரினங்களாகும். 
-ஆ)  செலாஜினெல்லா ஒத்தவித்துத்தன்மை கொண்ட ஒரு டெரிடோஃபைட் ஆகும்.
-இ) சைகஸ் பவழ வேர்கள் VAM கொண்டிருக்கின்றன.
-ஈ) பிரையோஃபைட்களில் முக்கிய தாவர உடலம் கேமீட்டக தாவரங்களாகும். அதேசமயம் டெரிடோஃபைட்களில் வித்தக தாவரங்களாகும்.
-உ) ஜிம்னோஸ்பெர்ம்களில் ஆண் மற்றும் பெண் கேமீட்டக தாவரங்கள் வித்தக தாவரங்களில் அமைந்துள்ள வித்தகங்களில் காணப்படுகின்றன.
-</t>
   </si>
   <si>
     <t>RNA மூலக்கூறை சூழ்ந்து புரத உறை காணப்படவில்லை</t>
@@ -2911,9 +2902,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L162"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3082,7 +3071,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>23</v>
@@ -3280,7 +3269,7 @@
         <v>774</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="I10" s="4"/>
       <c r="J10" s="4">
@@ -3493,7 +3482,7 @@
         <v>75</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="H16" s="4" t="s">
         <v>76</v>
@@ -3550,7 +3539,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>82</v>
@@ -3658,7 +3647,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>97</v>
@@ -3775,7 +3764,7 @@
         <v>2007</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>108</v>
@@ -3883,16 +3872,16 @@
         <v>2016</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>122</v>
       </c>
       <c r="G27" s="4" t="s">
+        <v>786</v>
+      </c>
+      <c r="H27" s="4" t="s">
         <v>787</v>
-      </c>
-      <c r="H27" s="4" t="s">
-        <v>788</v>
       </c>
       <c r="I27" s="4"/>
       <c r="J27" s="4">
@@ -3968,7 +3957,7 @@
       </c>
       <c r="I29" s="4"/>
       <c r="J29" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K29" s="4">
         <v>328</v>

</xml_diff>